<commit_message>
"galacticPubs::publish() [2022-09-13 09:31:31] "
</commit_message>
<xml_diff>
--- a/meta/acknowledgments.xlsx
+++ b/meta/acknowledgments.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgEcz00QpsuwiUS8ec83PcJeJqxQQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhIpWsjUrEjnI174ByDBHvzHXqKrQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -78,7 +78,7 @@
     <t>Classroom teacher expert advisory during lesson design process</t>
   </si>
   <si>
-    <t>Jade Griffiths</t>
+    <t>Jade Kennedy</t>
   </si>
   <si>
     <t>Mairehau High School</t>
@@ -151,11 +151,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
@@ -422,12 +420,12 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -448,7 +446,7 @@
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -459,26 +457,26 @@
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>

</xml_diff>